<commit_message>
add delete & public schedule
</commit_message>
<xml_diff>
--- a/flask/static/1 страница.xlsx
+++ b/flask/static/1 страница.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Серега\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F8A6B4-F053-48F4-B932-91EFCAB547DE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA9990F-33D2-4D93-B717-454EF0D82193}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="112">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -143,27 +143,12 @@
     <t>лек  лаб</t>
   </si>
   <si>
-    <t>лек  пр</t>
-  </si>
-  <si>
     <t>лек пр</t>
   </si>
   <si>
-    <t>Дискретная математика</t>
-  </si>
-  <si>
-    <t>Геометрия</t>
-  </si>
-  <si>
-    <t>дисциплина</t>
-  </si>
-  <si>
     <t>ФИО преподавателя</t>
   </si>
   <si>
-    <t>вид учебного занятия (лек,, практ., сем., лаб.)</t>
-  </si>
-  <si>
     <t>Наименование группы</t>
   </si>
   <si>
@@ -186,99 +171,27 @@
   </si>
   <si>
     <t xml:space="preserve">Алгебра      </t>
-  </si>
-  <si>
-    <t>Мальков И.М.</t>
   </si>
   <si>
     <t xml:space="preserve">Математический анализ        
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Алгебра и геометрия               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Алгебра и геометрия </t>
-  </si>
-  <si>
-    <t>Физика</t>
-  </si>
-  <si>
-    <t>Кампеева Е.Е.</t>
-  </si>
-  <si>
     <t>вид уч. занятия</t>
   </si>
   <si>
     <t>Дисциплина</t>
   </si>
   <si>
-    <t>Бочарова И.Н.</t>
-  </si>
-  <si>
-    <t>Максимов В.В.</t>
-  </si>
-  <si>
-    <t>Ефремова Е.А.</t>
-  </si>
-  <si>
-    <t>Андросова М.И.</t>
-  </si>
-  <si>
-    <t>Абрамова А.М.</t>
-  </si>
-  <si>
     <t>Основы проектной деятельности</t>
   </si>
   <si>
-    <t>Ситников С.И.</t>
-  </si>
-  <si>
-    <t>Антонов Ю.С.</t>
-  </si>
-  <si>
-    <t>Бубякин И.В.</t>
-  </si>
-  <si>
-    <t>Русский язык и культура речи</t>
-  </si>
-  <si>
-    <t>лек / пр</t>
-  </si>
-  <si>
-    <t>Программирование</t>
-  </si>
-  <si>
-    <t>Алгебра и теория чисел</t>
-  </si>
-  <si>
-    <t>Информатика</t>
-  </si>
-  <si>
-    <t>Экономика</t>
-  </si>
-  <si>
     <t>Элективные дисциплины по физической культуре и спорту</t>
   </si>
   <si>
-    <t>Старостина А.С.</t>
-  </si>
-  <si>
     <t>Акимов М.П.</t>
   </si>
   <si>
-    <t xml:space="preserve">Введение в сквозные цифровые технологии </t>
-  </si>
-  <si>
-    <t>Лыткин С.Д.</t>
-  </si>
-  <si>
-    <t>Бороев Р.Н.</t>
-  </si>
-  <si>
-    <t>Русский язык и культура речи**</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Введение в сквозные цифровые технологии</t>
   </si>
   <si>
@@ -288,76 +201,21 @@
     <t>**</t>
   </si>
   <si>
-    <t>Алексеев В.Н.</t>
-  </si>
-  <si>
-    <t>Афанасьева В.И.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Введение в математические пакеты прикладных программ </t>
-  </si>
-  <si>
-    <t>Слепцова Е.А.</t>
-  </si>
-  <si>
-    <t>Физика*</t>
-  </si>
-  <si>
-    <t>лаб/пр</t>
-  </si>
-  <si>
-    <t>Иностранный язык/</t>
-  </si>
-  <si>
     <t>Аналитическая геометрия</t>
   </si>
   <si>
     <t>СРС</t>
   </si>
   <si>
-    <t xml:space="preserve">Иностранный язык   </t>
-  </si>
-  <si>
     <t>ауд</t>
   </si>
   <si>
-    <t>ауд.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Русский язык и культура речи* </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Старостина А.С.  
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Русский язык и культура речи*  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Старостина А.С.  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Иностранный язык  </t>
   </si>
   <si>
-    <t>Б-МПО-22</t>
-  </si>
-  <si>
     <t>Б-М-22</t>
   </si>
   <si>
-    <t>Б-ПОИМ-22</t>
-  </si>
-  <si>
-    <t>Б-ПМИ-22-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Б-ПМИ-22-2 </t>
-  </si>
-  <si>
-    <t>Б-ИТСС-22</t>
-  </si>
-  <si>
     <t>2022-2023 уч. года</t>
   </si>
   <si>
@@ -436,27 +294,6 @@
     <t>26.06.2023 - 02.07.2023</t>
   </si>
   <si>
-    <t>Шарин Е.Ф.   Хохолов В.Б., Попова Т.С.</t>
-  </si>
-  <si>
-    <t>Шарин Е.Ф.   Неустроева Н.В., Попова Т.С.</t>
-  </si>
-  <si>
-    <t>Операционные системы</t>
-  </si>
-  <si>
-    <t>Общеуниверситетские дисциплины по выбору</t>
-  </si>
-  <si>
-    <t>Технология цифрового образования</t>
-  </si>
-  <si>
-    <t>Технология цифрового образования* Системное и прикладное программное обеспечение **</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Системное и прикладное программное обеспечение </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 25.01</t>
   </si>
   <si>
@@ -466,83 +303,19 @@
     <t>до</t>
   </si>
   <si>
-    <t xml:space="preserve"> 28.01</t>
-  </si>
-  <si>
-    <t>14.06.</t>
-  </si>
-  <si>
-    <t>Шарин Е.Ф.   Хохолов В.Б.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Введение в сквозные цифровые технологии*</t>
   </si>
   <si>
-    <t>Максимов В.В./Мальков И.М.</t>
-  </si>
-  <si>
     <t>Верховцев С.Д.</t>
   </si>
   <si>
-    <t>Технология цифрового образования*  ДВ.Технологии мультимедиа**</t>
-  </si>
-  <si>
-    <t>Максимов В.В./Ситников С.И.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Психология  </t>
-  </si>
-  <si>
-    <t>Психология воспитательных практик*
-Психология**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Психология воспитательных практик**</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Психология воспитательных практик*</t>
-  </si>
-  <si>
-    <t>330  326</t>
-  </si>
-  <si>
     <t>Программирование *,**</t>
   </si>
   <si>
-    <t>424   430</t>
-  </si>
-  <si>
-    <t>424  430 432</t>
-  </si>
-  <si>
-    <t>326  330  353</t>
-  </si>
-  <si>
     <t>четверг</t>
   </si>
   <si>
-    <t>\</t>
-  </si>
-  <si>
-    <t>Программирование**</t>
-  </si>
-  <si>
-    <t>Информатика*</t>
-  </si>
-  <si>
-    <t>ДВ. Технологии мультимедиа/Компьютерная графика</t>
-  </si>
-  <si>
-    <t>224 а/424</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 14.06</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 06.06</t>
-  </si>
-  <si>
-    <t>31.05</t>
   </si>
   <si>
     <t>Григорьев В.В.
@@ -554,35 +327,56 @@
 Ларионова И.Г.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Основы медицинских знаний</t>
-  </si>
-  <si>
-    <t>Гольдерова А.С.</t>
-  </si>
-  <si>
-    <t>Компьютерная графика**</t>
-  </si>
-  <si>
-    <t>Находкина И.И.</t>
-  </si>
-  <si>
     <t>Неустроева Т.К.</t>
   </si>
   <si>
-    <t xml:space="preserve">Григорьев В.В. </t>
-  </si>
-  <si>
     <t>Делахов  Д.А.</t>
   </si>
   <si>
-    <t xml:space="preserve">Математический  анализ 
-разбить на 3 пары в одно время по преподавателям </t>
-  </si>
-  <si>
     <t>Р   А   С   П   И   С   А   Н   И   Е       З    А    Н    Я    Т    И    Й       И М И           на 2 полугодие    2022-2023 уч.года</t>
   </si>
   <si>
     <t>1                курс</t>
+  </si>
+  <si>
+    <t>Спортивный</t>
+  </si>
+  <si>
+    <t>Шарин Е.Ф. 
+Хохолов В.Б. 
+Попова Т.С.</t>
+  </si>
+  <si>
+    <t>Шарин Е.Ф.
+ Хохолов В.Б.</t>
+  </si>
+  <si>
+    <t>Шарин Е.Ф. 
+Неустроева Н.В. 
+Попова Т.С.</t>
+  </si>
+  <si>
+    <t>326 
+ 330 
+ 353</t>
+  </si>
+  <si>
+    <t>330 
+ 326</t>
+  </si>
+  <si>
+    <t>424 
+  430</t>
+  </si>
+  <si>
+    <t>424 
+ 430 
+432</t>
+  </si>
+  <si>
+    <t>326 
+ 330
+ 353</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1141,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1728,9 +1522,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2293,10 +2084,10 @@
   <dimension ref="A1:AE53"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="41" zoomScaleNormal="50" zoomScaleSheetLayoutView="41" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:V2"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.2"/>
@@ -2307,25 +2098,25 @@
     <col min="4" max="4" width="30.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="45.7109375" style="194" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" style="194" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" style="194" customWidth="1"/>
-    <col min="11" max="11" width="45.7109375" style="194" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" style="194" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="194" customWidth="1"/>
+    <col min="7" max="7" width="45.7109375" style="193" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="193" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" style="193" customWidth="1"/>
+    <col min="11" max="11" width="45.7109375" style="193" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" style="193" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="193" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" style="123" customWidth="1"/>
     <col min="15" max="15" width="45.7109375" style="77" customWidth="1"/>
     <col min="16" max="16" width="30.7109375" style="77" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" style="77" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="195" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="194" customWidth="1"/>
     <col min="19" max="19" width="45.7109375" style="77" customWidth="1"/>
     <col min="20" max="20" width="30.7109375" style="77" customWidth="1"/>
     <col min="21" max="21" width="10.7109375" style="77" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" style="179" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="178" customWidth="1"/>
     <col min="23" max="23" width="42.85546875" style="19" customWidth="1"/>
     <col min="24" max="24" width="30.7109375" style="19" customWidth="1"/>
     <col min="25" max="25" width="10.7109375" style="19" customWidth="1"/>
-    <col min="26" max="26" width="10.7109375" style="161" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" style="160" customWidth="1"/>
     <col min="27" max="27" width="5.42578125" style="83" customWidth="1"/>
     <col min="28" max="28" width="35.28515625" style="1" customWidth="1"/>
     <col min="29" max="256" width="8.85546875" style="4"/>
@@ -3719,229 +3510,149 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="202" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="202"/>
-      <c r="C1" s="202"/>
-      <c r="D1" s="202"/>
-      <c r="E1" s="202"/>
-      <c r="F1" s="202"/>
-      <c r="G1" s="202"/>
-      <c r="H1" s="202"/>
-      <c r="I1" s="202"/>
-      <c r="J1" s="202"/>
-      <c r="K1" s="202"/>
-      <c r="L1" s="202"/>
-      <c r="M1" s="202"/>
-      <c r="N1" s="202"/>
-      <c r="O1" s="202"/>
-      <c r="P1" s="202"/>
-      <c r="Q1" s="202"/>
-      <c r="R1" s="202"/>
-      <c r="S1" s="181"/>
-      <c r="T1" s="181"/>
-      <c r="U1" s="181"/>
+      <c r="A1" s="201" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
+      <c r="M1" s="201"/>
+      <c r="N1" s="201"/>
+      <c r="O1" s="201"/>
+      <c r="P1" s="201"/>
+      <c r="Q1" s="201"/>
+      <c r="R1" s="201"/>
+      <c r="S1" s="180"/>
+      <c r="T1" s="180"/>
+      <c r="U1" s="180"/>
       <c r="V1" s="101"/>
-      <c r="W1" s="152"/>
-      <c r="X1" s="152"/>
-      <c r="Y1" s="152"/>
+      <c r="W1" s="151"/>
+      <c r="X1" s="151"/>
+      <c r="Y1" s="151"/>
       <c r="Z1" s="101"/>
       <c r="AA1" s="50"/>
     </row>
     <row r="2" spans="1:28" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="203" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="204"/>
-      <c r="C2" s="204"/>
-      <c r="D2" s="204"/>
-      <c r="E2" s="204"/>
-      <c r="F2" s="204"/>
-      <c r="G2" s="204"/>
-      <c r="H2" s="204"/>
-      <c r="I2" s="204"/>
-      <c r="J2" s="204"/>
-      <c r="K2" s="204"/>
-      <c r="L2" s="204"/>
-      <c r="M2" s="204"/>
-      <c r="N2" s="204"/>
-      <c r="O2" s="204"/>
-      <c r="P2" s="204"/>
-      <c r="Q2" s="204"/>
-      <c r="R2" s="204"/>
-      <c r="S2" s="205"/>
-      <c r="T2" s="205"/>
-      <c r="U2" s="205"/>
-      <c r="V2" s="205"/>
-      <c r="W2" s="163"/>
-      <c r="X2" s="163"/>
-      <c r="Y2" s="163"/>
-      <c r="Z2" s="164"/>
+      <c r="A2" s="202" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="203"/>
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="203"/>
+      <c r="H2" s="203"/>
+      <c r="I2" s="203"/>
+      <c r="J2" s="203"/>
+      <c r="K2" s="203"/>
+      <c r="L2" s="203"/>
+      <c r="M2" s="203"/>
+      <c r="N2" s="203"/>
+      <c r="O2" s="203"/>
+      <c r="P2" s="203"/>
+      <c r="Q2" s="203"/>
+      <c r="R2" s="203"/>
+      <c r="S2" s="204"/>
+      <c r="T2" s="204"/>
+      <c r="U2" s="204"/>
+      <c r="V2" s="204"/>
+      <c r="W2" s="162"/>
+      <c r="X2" s="162"/>
+      <c r="Y2" s="162"/>
+      <c r="Z2" s="163"/>
       <c r="AB2" s="27" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:28" s="31" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28"/>
-      <c r="B3" s="162"/>
+      <c r="B3" s="161"/>
       <c r="C3" s="44" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="173" t="s">
-        <v>144</v>
-      </c>
-      <c r="F3" s="174" t="s">
-        <v>145</v>
-      </c>
-      <c r="G3" s="79" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="80" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="168" t="s">
-        <v>144</v>
-      </c>
-      <c r="J3" s="184" t="s">
-        <v>145</v>
-      </c>
-      <c r="K3" s="183" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" s="80" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" s="168" t="s">
-        <v>144</v>
-      </c>
-      <c r="N3" s="184" t="s">
-        <v>145</v>
-      </c>
-      <c r="O3" s="185" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" s="186" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q3" s="180" t="s">
-        <v>144</v>
-      </c>
-      <c r="R3" s="187" t="s">
-        <v>145</v>
-      </c>
-      <c r="S3" s="176" t="s">
-        <v>46</v>
-      </c>
-      <c r="T3" s="177" t="s">
-        <v>47</v>
-      </c>
-      <c r="U3" s="182" t="s">
-        <v>144</v>
-      </c>
-      <c r="V3" s="188" t="s">
-        <v>145</v>
-      </c>
-      <c r="W3" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="X3" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y3" s="166" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z3" s="167" t="s">
-        <v>145</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E3" s="172" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="173" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="79"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="167"/>
+      <c r="J3" s="183"/>
+      <c r="K3" s="182"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="167"/>
+      <c r="N3" s="183"/>
+      <c r="O3" s="184"/>
+      <c r="P3" s="185"/>
+      <c r="Q3" s="179"/>
+      <c r="R3" s="186"/>
+      <c r="S3" s="175"/>
+      <c r="T3" s="176"/>
+      <c r="U3" s="181"/>
+      <c r="V3" s="187"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="165"/>
+      <c r="Z3" s="166"/>
       <c r="AA3" s="51"/>
       <c r="AB3" s="19" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:28" s="49" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32"/>
       <c r="B4" s="33"/>
       <c r="C4" s="47" t="s">
-        <v>105</v>
+        <v>62</v>
       </c>
       <c r="D4" s="48">
         <v>20</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
       <c r="F4" s="94" t="s">
-        <v>169</v>
-      </c>
-      <c r="G4" s="171" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="74">
-        <v>19</v>
-      </c>
-      <c r="I4" s="196" t="s">
-        <v>143</v>
-      </c>
-      <c r="J4" s="145" t="s">
-        <v>170</v>
-      </c>
-      <c r="K4" s="110" t="s">
-        <v>106</v>
-      </c>
-      <c r="L4" s="74">
-        <v>18</v>
-      </c>
-      <c r="M4" s="74" t="s">
-        <v>143</v>
-      </c>
-      <c r="N4" s="189">
-        <v>44726</v>
-      </c>
-      <c r="O4" s="171" t="s">
-        <v>107</v>
-      </c>
-      <c r="P4" s="74">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="74" t="s">
-        <v>143</v>
-      </c>
-      <c r="R4" s="190" t="s">
-        <v>147</v>
-      </c>
-      <c r="S4" s="110" t="s">
-        <v>108</v>
-      </c>
-      <c r="T4" s="74">
-        <v>17</v>
-      </c>
-      <c r="U4" s="74" t="s">
-        <v>143</v>
-      </c>
-      <c r="V4" s="190" t="s">
-        <v>147</v>
-      </c>
-      <c r="W4" s="35" t="s">
-        <v>109</v>
-      </c>
-      <c r="X4" s="36">
-        <v>18</v>
-      </c>
-      <c r="Y4" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z4" s="175" t="s">
-        <v>171</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="G4" s="170"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="195"/>
+      <c r="J4" s="144"/>
+      <c r="K4" s="110"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="188"/>
+      <c r="O4" s="170"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="189"/>
+      <c r="S4" s="110"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
+      <c r="V4" s="189"/>
+      <c r="W4" s="35"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="34"/>
+      <c r="Z4" s="174"/>
       <c r="AA4" s="51" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="AB4" s="26" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:28" s="31" customFormat="1" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3952,160 +3663,98 @@
         <v>23</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E5" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="99" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="99" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" s="192" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="75" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="144" t="s">
-        <v>97</v>
-      </c>
-      <c r="K5" s="111" t="s">
-        <v>61</v>
-      </c>
-      <c r="L5" s="75" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="N5" s="191" t="s">
-        <v>97</v>
-      </c>
-      <c r="O5" s="192" t="s">
-        <v>61</v>
-      </c>
-      <c r="P5" s="75" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q5" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="R5" s="144" t="s">
-        <v>97</v>
-      </c>
-      <c r="S5" s="111" t="s">
-        <v>61</v>
-      </c>
-      <c r="T5" s="75" t="s">
-        <v>44</v>
-      </c>
-      <c r="U5" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="V5" s="100" t="s">
-        <v>97</v>
-      </c>
-      <c r="W5" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="X5" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y5" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z5" s="103" t="s">
-        <v>98</v>
-      </c>
+      <c r="G5" s="191"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="143"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="190"/>
+      <c r="O5" s="191"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="143"/>
+      <c r="S5" s="111"/>
+      <c r="T5" s="75"/>
+      <c r="U5" s="75"/>
+      <c r="V5" s="100"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="40"/>
+      <c r="Y5" s="40"/>
+      <c r="Z5" s="103"/>
       <c r="AA5" s="52" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="AB5" s="19" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="198" t="s">
+      <c r="A6" s="197" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="53" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="128" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="D6" s="129"/>
       <c r="E6" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="131"/>
-      <c r="G6" s="128" t="s">
-        <v>48</v>
-      </c>
+      <c r="F6" s="131">
+        <v>353</v>
+      </c>
+      <c r="G6" s="128"/>
       <c r="H6" s="130"/>
-      <c r="I6" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="I6" s="130"/>
       <c r="J6" s="132"/>
-      <c r="K6" s="128" t="s">
-        <v>48</v>
-      </c>
+      <c r="K6" s="128"/>
       <c r="L6" s="129"/>
-      <c r="M6" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="M6" s="130"/>
       <c r="N6" s="132"/>
-      <c r="O6" s="128" t="s">
-        <v>96</v>
-      </c>
+      <c r="O6" s="128"/>
       <c r="P6" s="129"/>
-      <c r="Q6" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="Q6" s="130"/>
       <c r="R6" s="132"/>
-      <c r="S6" s="133" t="s">
-        <v>96</v>
-      </c>
+      <c r="S6" s="133"/>
       <c r="T6" s="129"/>
-      <c r="U6" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="U6" s="130"/>
       <c r="V6" s="130"/>
-      <c r="W6" s="153" t="s">
-        <v>48</v>
-      </c>
-      <c r="X6" s="129" t="s">
+      <c r="W6" s="152"/>
+      <c r="X6" s="129"/>
+      <c r="Y6" s="129"/>
+      <c r="Z6" s="153"/>
+      <c r="AA6" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB6" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="Y6" s="129" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z6" s="154">
-        <v>457</v>
-      </c>
-      <c r="AA6" s="86" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB6" s="10" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="7" spans="1:28" s="55" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="199"/>
+      <c r="A7" s="198"/>
       <c r="B7" s="90" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>34</v>
@@ -4113,83 +3762,43 @@
       <c r="F7" s="106">
         <v>430</v>
       </c>
-      <c r="G7" s="54" t="s">
-        <v>152</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" s="112">
-        <v>330</v>
-      </c>
-      <c r="K7" s="54" t="s">
-        <v>141</v>
-      </c>
-      <c r="L7" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="M7" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" s="112">
-        <v>330</v>
-      </c>
-      <c r="O7" s="20" t="s">
+      <c r="G7" s="54"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="112"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="112"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="113"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="98"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="154"/>
+      <c r="AA7" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="P7" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q7" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="R7" s="113">
-        <v>449</v>
-      </c>
-      <c r="S7" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="T7" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="U7" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="V7" s="98">
-        <v>424</v>
-      </c>
-      <c r="W7" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="X7" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y7" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z7" s="155">
-        <v>540</v>
-      </c>
-      <c r="AA7" s="68" t="s">
-        <v>85</v>
-      </c>
       <c r="AB7" s="10" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="199"/>
+      <c r="A8" s="198"/>
       <c r="B8" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>33</v>
@@ -4197,151 +3806,79 @@
       <c r="F8" s="106">
         <v>330</v>
       </c>
-      <c r="G8" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="120">
-        <v>430</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="L8" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="M8" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" s="113">
-        <v>432</v>
-      </c>
-      <c r="O8" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="P8" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q8" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="R8" s="113">
-        <v>330</v>
-      </c>
-      <c r="S8" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="T8" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="U8" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="V8" s="22">
-        <v>330</v>
-      </c>
-      <c r="W8" s="165"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="113"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="113"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="164"/>
       <c r="X8" s="25"/>
       <c r="Y8" s="25"/>
       <c r="Z8" s="113"/>
       <c r="AA8" s="86" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="AB8" s="10" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="199"/>
+      <c r="A9" s="198"/>
       <c r="B9" s="66" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="F9" s="106">
         <v>551</v>
       </c>
-      <c r="G9" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="112">
-        <v>461</v>
-      </c>
-      <c r="K9" s="54" t="s">
-        <v>101</v>
-      </c>
-      <c r="L9" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="M9" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="N9" s="112">
-        <v>461</v>
-      </c>
-      <c r="O9" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="P9" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q9" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="R9" s="112">
-        <v>461</v>
-      </c>
-      <c r="S9" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="T9" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="U9" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="V9" s="98">
-        <v>461</v>
-      </c>
-      <c r="W9" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="X9" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y9" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z9" s="155">
-        <v>461</v>
-      </c>
+      <c r="G9" s="54"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="112"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="112"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="112"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="98"/>
+      <c r="W9" s="54"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="154"/>
       <c r="AA9" s="86" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="AB9" s="10" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="199"/>
+      <c r="A10" s="198"/>
       <c r="B10" s="59" t="s">
         <v>36</v>
       </c>
@@ -4370,14 +3907,14 @@
       <c r="Y10" s="14"/>
       <c r="Z10" s="96"/>
       <c r="AA10" s="68" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="AB10" s="10" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="201"/>
+      <c r="A11" s="200"/>
       <c r="B11" s="60" t="s">
         <v>37</v>
       </c>
@@ -4406,300 +3943,182 @@
       <c r="Y11" s="11"/>
       <c r="Z11" s="95"/>
       <c r="AA11" s="68" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="AB11" s="10" t="s">
-        <v>118</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="198" t="s">
+      <c r="A12" s="197" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="53" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="128" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="D12" s="129"/>
       <c r="E12" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="131"/>
-      <c r="G12" s="128" t="s">
-        <v>48</v>
-      </c>
+      <c r="F12" s="131">
+        <v>353</v>
+      </c>
+      <c r="G12" s="128"/>
       <c r="H12" s="130"/>
-      <c r="I12" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="I12" s="130"/>
       <c r="J12" s="132"/>
-      <c r="K12" s="128" t="s">
-        <v>48</v>
-      </c>
+      <c r="K12" s="128"/>
       <c r="L12" s="129"/>
-      <c r="M12" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="M12" s="130"/>
       <c r="N12" s="132"/>
-      <c r="O12" s="128" t="s">
-        <v>96</v>
-      </c>
+      <c r="O12" s="128"/>
       <c r="P12" s="129"/>
-      <c r="Q12" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="Q12" s="130"/>
       <c r="R12" s="132"/>
-      <c r="S12" s="133" t="s">
-        <v>96</v>
-      </c>
+      <c r="S12" s="133"/>
       <c r="T12" s="129"/>
-      <c r="U12" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="U12" s="130"/>
       <c r="V12" s="130"/>
-      <c r="W12" s="153" t="s">
-        <v>48</v>
-      </c>
-      <c r="X12" s="129" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y12" s="129" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z12" s="154">
-        <v>457</v>
-      </c>
+      <c r="W12" s="152"/>
+      <c r="X12" s="129"/>
+      <c r="Y12" s="129"/>
+      <c r="Z12" s="153"/>
       <c r="AA12" s="68" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="AB12" s="10" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="199"/>
+      <c r="A13" s="198"/>
       <c r="B13" s="59" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>172</v>
+        <v>97</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="93" t="s">
-        <v>158</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="I13" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="113">
-        <v>426</v>
-      </c>
-      <c r="K13" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="L13" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="M13" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="N13" s="146">
-        <v>555</v>
-      </c>
-      <c r="O13" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="P13" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q13" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="R13" s="93" t="s">
-        <v>158</v>
-      </c>
-      <c r="S13" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="T13" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="U13" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="V13" s="93" t="s">
-        <v>158</v>
-      </c>
-      <c r="W13" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="X13" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y13" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z13" s="70">
-        <v>519</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="145"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="93"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="93"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="25"/>
+      <c r="Y13" s="22"/>
+      <c r="Z13" s="70"/>
       <c r="AA13" s="68" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="AB13" s="10" t="s">
-        <v>120</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="199"/>
+      <c r="A14" s="198"/>
       <c r="B14" s="59" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>34</v>
       </c>
       <c r="F14" s="113" t="s">
-        <v>161</v>
+        <v>110</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>
       <c r="J14" s="113"/>
-      <c r="K14" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="L14" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="M14" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="N14" s="113">
-        <v>555</v>
-      </c>
-      <c r="O14" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="P14" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q14" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="R14" s="113" t="s">
-        <v>161</v>
-      </c>
-      <c r="S14" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="T14" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="U14" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="V14" s="113" t="s">
-        <v>161</v>
-      </c>
-      <c r="W14" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="X14" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y14" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z14" s="70">
-        <v>449</v>
-      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="113"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="113"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="113"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="22"/>
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="70"/>
       <c r="AA14" s="68" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="AB14" s="10" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="199"/>
+      <c r="A15" s="198"/>
       <c r="B15" s="70" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="82"/>
       <c r="D15" s="22"/>
       <c r="E15" s="63"/>
-      <c r="F15" s="146"/>
+      <c r="F15" s="145"/>
       <c r="G15" s="20"/>
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
       <c r="J15" s="113"/>
-      <c r="K15" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="L15" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="M15" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="N15" s="146">
-        <v>430</v>
-      </c>
-      <c r="O15" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="P15" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q15" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="R15" s="115">
-        <v>330</v>
-      </c>
-      <c r="S15" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="T15" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="U15" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="V15" s="146">
-        <v>330</v>
-      </c>
+      <c r="K15" s="20"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="145"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="115"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="145"/>
       <c r="W15" s="20"/>
       <c r="X15" s="22"/>
       <c r="Y15" s="24"/>
       <c r="Z15" s="113"/>
       <c r="AA15" s="68" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="AB15" s="10" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="199"/>
+      <c r="A16" s="198"/>
       <c r="B16" s="59" t="s">
         <v>36</v>
       </c>
@@ -4714,28 +4133,28 @@
       <c r="K16" s="14"/>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
-      <c r="N16" s="146"/>
+      <c r="N16" s="145"/>
       <c r="O16" s="92"/>
       <c r="P16" s="25"/>
-      <c r="Q16" s="148"/>
-      <c r="R16" s="147"/>
+      <c r="Q16" s="147"/>
+      <c r="R16" s="146"/>
       <c r="S16" s="17"/>
       <c r="T16" s="25"/>
       <c r="U16" s="22"/>
       <c r="V16" s="22"/>
-      <c r="W16" s="156"/>
+      <c r="W16" s="155"/>
       <c r="X16" s="22"/>
       <c r="Y16" s="93"/>
       <c r="Z16" s="113"/>
       <c r="AA16" s="68" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="AB16" s="10" t="s">
-        <v>123</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="201"/>
+      <c r="A17" s="200"/>
       <c r="B17" s="60"/>
       <c r="C17" s="54"/>
       <c r="D17" s="25"/>
@@ -4762,304 +4181,188 @@
       <c r="Y17" s="11"/>
       <c r="Z17" s="95"/>
       <c r="AA17" s="68" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="AB17" s="10" t="s">
-        <v>124</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="207" t="s">
+      <c r="A18" s="206" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="53" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="128" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="D18" s="129"/>
       <c r="E18" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="131"/>
-      <c r="G18" s="128" t="s">
-        <v>48</v>
-      </c>
+      <c r="F18" s="131">
+        <v>353</v>
+      </c>
+      <c r="G18" s="128"/>
       <c r="H18" s="130"/>
-      <c r="I18" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="I18" s="130"/>
       <c r="J18" s="132"/>
-      <c r="K18" s="128" t="s">
-        <v>48</v>
-      </c>
+      <c r="K18" s="128"/>
       <c r="L18" s="129"/>
-      <c r="M18" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="M18" s="130"/>
       <c r="N18" s="132"/>
-      <c r="O18" s="128" t="s">
-        <v>96</v>
-      </c>
+      <c r="O18" s="128"/>
       <c r="P18" s="129"/>
-      <c r="Q18" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="Q18" s="130"/>
       <c r="R18" s="132"/>
-      <c r="S18" s="133" t="s">
-        <v>96</v>
-      </c>
+      <c r="S18" s="133"/>
       <c r="T18" s="129"/>
-      <c r="U18" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="U18" s="130"/>
       <c r="V18" s="130"/>
-      <c r="W18" s="153" t="s">
-        <v>48</v>
-      </c>
+      <c r="W18" s="152"/>
       <c r="X18" s="129"/>
-      <c r="Y18" s="129" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z18" s="154"/>
+      <c r="Y18" s="129"/>
+      <c r="Z18" s="153"/>
       <c r="AA18" s="68" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="AB18" s="10" t="s">
-        <v>125</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="208"/>
+      <c r="A19" s="207"/>
       <c r="B19" s="56" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="E19" s="24" t="s">
         <v>38</v>
       </c>
       <c r="F19" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="G19" s="54" t="s">
-        <v>174</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="I19" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J19" s="115">
-        <v>328</v>
-      </c>
-      <c r="K19" s="54" t="s">
-        <v>174</v>
-      </c>
-      <c r="L19" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="M19" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="N19" s="115">
-        <v>328</v>
-      </c>
-      <c r="O19" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="P19" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q19" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="R19" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="S19" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="T19" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="U19" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="V19" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="W19" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="X19" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y19" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z19" s="96">
-        <v>540</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="G19" s="54"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="115"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="115"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="66"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="66"/>
+      <c r="W19" s="54"/>
+      <c r="X19" s="22"/>
+      <c r="Y19" s="22"/>
+      <c r="Z19" s="96"/>
       <c r="AA19" s="68" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="AB19" s="10" t="s">
-        <v>126</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="208"/>
+      <c r="A20" s="207"/>
       <c r="B20" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="157" t="s">
-        <v>77</v>
+      <c r="C20" s="156" t="s">
+        <v>53</v>
       </c>
       <c r="D20" s="137"/>
       <c r="E20" s="134" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="138"/>
-      <c r="G20" s="157" t="s">
-        <v>77</v>
-      </c>
+      <c r="F20" s="105" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="156"/>
       <c r="H20" s="137"/>
-      <c r="I20" s="134" t="s">
-        <v>35</v>
-      </c>
-      <c r="J20" s="139"/>
-      <c r="K20" s="172" t="s">
-        <v>77</v>
-      </c>
+      <c r="I20" s="134"/>
+      <c r="J20" s="138"/>
+      <c r="K20" s="171"/>
       <c r="L20" s="137"/>
-      <c r="M20" s="134" t="s">
-        <v>35</v>
-      </c>
-      <c r="N20" s="139"/>
-      <c r="O20" s="157" t="s">
-        <v>77</v>
-      </c>
+      <c r="M20" s="134"/>
+      <c r="N20" s="138"/>
+      <c r="O20" s="156"/>
       <c r="P20" s="137"/>
-      <c r="Q20" s="134" t="s">
-        <v>35</v>
-      </c>
-      <c r="R20" s="140"/>
-      <c r="S20" s="172" t="s">
-        <v>77</v>
-      </c>
+      <c r="Q20" s="134"/>
+      <c r="R20" s="139"/>
+      <c r="S20" s="171"/>
       <c r="T20" s="137"/>
-      <c r="U20" s="134" t="s">
-        <v>35</v>
-      </c>
-      <c r="V20" s="140"/>
-      <c r="W20" s="157" t="s">
-        <v>77</v>
-      </c>
+      <c r="U20" s="134"/>
+      <c r="V20" s="139"/>
+      <c r="W20" s="156"/>
       <c r="X20" s="137"/>
-      <c r="Y20" s="134" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z20" s="139"/>
-      <c r="AA20" s="170" t="s">
-        <v>86</v>
+      <c r="Y20" s="134"/>
+      <c r="Z20" s="138"/>
+      <c r="AA20" s="169" t="s">
+        <v>57</v>
       </c>
       <c r="AB20" s="10" t="s">
-        <v>127</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="208"/>
+      <c r="A21" s="207"/>
       <c r="B21" s="59" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="149">
+        <v>39</v>
+      </c>
+      <c r="F21" s="148">
         <v>551</v>
       </c>
-      <c r="G21" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="H21" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J21" s="96">
-        <v>328</v>
-      </c>
-      <c r="K21" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="L21" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="N21" s="96">
-        <v>328</v>
-      </c>
-      <c r="O21" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="P21" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q21" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="R21" s="96">
-        <v>330</v>
-      </c>
-      <c r="S21" s="102" t="s">
-        <v>57</v>
-      </c>
-      <c r="T21" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="U21" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="V21" s="96">
-        <v>330</v>
-      </c>
-      <c r="W21" s="54" t="s">
-        <v>76</v>
-      </c>
-      <c r="X21" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y21" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z21" s="96">
-        <v>555</v>
-      </c>
+      <c r="G21" s="54"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="96"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="96"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="96"/>
+      <c r="S21" s="102"/>
+      <c r="T21" s="25"/>
+      <c r="U21" s="63"/>
+      <c r="V21" s="96"/>
+      <c r="W21" s="54"/>
+      <c r="X21" s="22"/>
+      <c r="Y21" s="22"/>
+      <c r="Z21" s="96"/>
       <c r="AA21" s="68" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="AB21" s="10" t="s">
-        <v>128</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="208"/>
+      <c r="A22" s="207"/>
       <c r="B22" s="59" t="s">
         <v>36</v>
       </c>
@@ -5067,30 +4370,14 @@
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="109"/>
-      <c r="G22" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="I22" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="J22" s="113">
-        <v>328</v>
-      </c>
-      <c r="K22" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="L22" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="M22" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" s="113">
-        <v>328</v>
-      </c>
+      <c r="G22" s="54"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="113"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="113"/>
       <c r="O22" s="20"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="22"/>
@@ -5104,14 +4391,14 @@
       <c r="Y22" s="25"/>
       <c r="Z22" s="96"/>
       <c r="AA22" s="68" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="AB22" s="10" t="s">
-        <v>129</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="209"/>
+      <c r="A23" s="208"/>
       <c r="B23" s="60" t="s">
         <v>37</v>
       </c>
@@ -5126,7 +4413,7 @@
       <c r="K23" s="15"/>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
-      <c r="N23" s="144"/>
+      <c r="N23" s="143"/>
       <c r="O23" s="16"/>
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
@@ -5140,88 +4427,66 @@
       <c r="Y23" s="11"/>
       <c r="Z23" s="95"/>
       <c r="AA23" s="68" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="AB23" s="10" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="210" t="s">
-        <v>163</v>
+      <c r="A24" s="209" t="s">
+        <v>95</v>
       </c>
       <c r="B24" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="141" t="s">
-        <v>48</v>
+      <c r="C24" s="140" t="s">
+        <v>43</v>
       </c>
       <c r="D24" s="136"/>
-      <c r="E24" s="142" t="s">
+      <c r="E24" s="141" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="143"/>
-      <c r="G24" s="128" t="s">
-        <v>96</v>
-      </c>
+      <c r="F24" s="142">
+        <v>353</v>
+      </c>
+      <c r="G24" s="128"/>
       <c r="H24" s="130"/>
-      <c r="I24" s="130" t="s">
-        <v>72</v>
-      </c>
+      <c r="I24" s="130"/>
       <c r="J24" s="132"/>
-      <c r="K24" s="128" t="s">
-        <v>48</v>
-      </c>
+      <c r="K24" s="128"/>
       <c r="L24" s="129"/>
-      <c r="M24" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="M24" s="130"/>
       <c r="N24" s="132"/>
-      <c r="O24" s="128" t="s">
-        <v>93</v>
-      </c>
+      <c r="O24" s="128"/>
       <c r="P24" s="130"/>
-      <c r="Q24" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="Q24" s="130"/>
       <c r="R24" s="132"/>
-      <c r="S24" s="135" t="s">
-        <v>48</v>
-      </c>
-      <c r="T24" s="136" t="s">
-        <v>79</v>
-      </c>
-      <c r="U24" s="136" t="s">
-        <v>35</v>
-      </c>
+      <c r="S24" s="135"/>
+      <c r="T24" s="136"/>
+      <c r="U24" s="136"/>
       <c r="V24" s="136"/>
-      <c r="W24" s="157" t="s">
-        <v>48</v>
-      </c>
-      <c r="X24" s="134" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y24" s="158" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z24" s="140"/>
+      <c r="W24" s="156"/>
+      <c r="X24" s="134"/>
+      <c r="Y24" s="157"/>
+      <c r="Z24" s="139"/>
       <c r="AA24" s="68" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="AB24" s="10" t="s">
-        <v>131</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="211"/>
+      <c r="A25" s="210"/>
       <c r="B25" s="59" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E25" s="22" t="s">
         <v>33</v>
@@ -5229,83 +4494,43 @@
       <c r="F25" s="93">
         <v>353</v>
       </c>
-      <c r="G25" s="150" t="s">
-        <v>155</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="I25" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J25" s="113">
-        <v>326</v>
-      </c>
-      <c r="K25" s="150" t="s">
-        <v>155</v>
-      </c>
-      <c r="L25" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="M25" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="N25" s="113">
-        <v>326</v>
-      </c>
-      <c r="O25" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="P25" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q25" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="R25" s="113">
-        <v>424</v>
-      </c>
-      <c r="S25" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="T25" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="U25" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="V25" s="22">
-        <v>426</v>
-      </c>
-      <c r="W25" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="X25" s="93" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y25" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z25" s="96">
-        <v>540</v>
-      </c>
+      <c r="G25" s="149"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="113"/>
+      <c r="K25" s="149"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="113"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="113"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="22"/>
+      <c r="W25" s="20"/>
+      <c r="X25" s="93"/>
+      <c r="Y25" s="22"/>
+      <c r="Z25" s="96"/>
       <c r="AA25" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB25" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="AB25" s="10" t="s">
-        <v>132</v>
-      </c>
     </row>
     <row r="26" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="211"/>
+      <c r="A26" s="210"/>
       <c r="B26" s="59" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E26" s="22" t="s">
         <v>34</v>
@@ -5313,151 +4538,79 @@
       <c r="F26" s="93">
         <v>353</v>
       </c>
-      <c r="G26" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="H26" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="I26" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="J26" s="96">
-        <v>455</v>
-      </c>
-      <c r="K26" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="L26" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="M26" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="N26" s="113">
-        <v>430</v>
-      </c>
-      <c r="O26" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="P26" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q26" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="R26" s="113">
-        <v>424</v>
-      </c>
-      <c r="S26" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="T26" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="U26" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="V26" s="22">
-        <v>559</v>
-      </c>
-      <c r="W26" s="156" t="s">
-        <v>41</v>
-      </c>
-      <c r="X26" s="93" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y26" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z26" s="96">
-        <v>540</v>
-      </c>
+      <c r="G26" s="20"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="96"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="113"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="113"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="22"/>
+      <c r="U26" s="22"/>
+      <c r="V26" s="22"/>
+      <c r="W26" s="155"/>
+      <c r="X26" s="93"/>
+      <c r="Y26" s="93"/>
+      <c r="Z26" s="96"/>
       <c r="AA26" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB26" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="AB26" s="10" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="27" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="211"/>
+      <c r="A27" s="210"/>
       <c r="B27" s="59" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="82" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="E27" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="146" t="s">
-        <v>160</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="H27" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="I27" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="J27" s="115">
-        <v>447</v>
-      </c>
-      <c r="K27" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="L27" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="M27" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="N27" s="115">
-        <v>455</v>
-      </c>
-      <c r="O27" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="P27" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q27" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="R27" s="146" t="s">
-        <v>160</v>
-      </c>
-      <c r="S27" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="T27" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="U27" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="V27" s="146" t="s">
-        <v>160</v>
-      </c>
+      <c r="F27" s="145" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" s="20"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="115"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="115"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="145"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
+      <c r="V27" s="145"/>
       <c r="W27" s="54"/>
       <c r="X27" s="22"/>
       <c r="Y27" s="22"/>
       <c r="Z27" s="113"/>
       <c r="AA27" s="68" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="AB27" s="10" t="s">
-        <v>134</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="211"/>
+      <c r="A28" s="210"/>
       <c r="B28" s="59" t="s">
         <v>36</v>
       </c>
@@ -5465,30 +4618,14 @@
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
       <c r="F28" s="93"/>
-      <c r="G28" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="H28" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="I28" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="J28" s="113">
-        <v>455</v>
-      </c>
-      <c r="K28" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="L28" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="M28" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="N28" s="121">
-        <v>455</v>
-      </c>
+      <c r="G28" s="20"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="113"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="121"/>
       <c r="O28" s="54"/>
       <c r="P28" s="25"/>
       <c r="Q28" s="25"/>
@@ -5502,14 +4639,14 @@
       <c r="Y28" s="22"/>
       <c r="Z28" s="113"/>
       <c r="AA28" s="68" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="AB28" s="10" t="s">
-        <v>135</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:31" s="55" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="212"/>
+      <c r="A29" s="211"/>
       <c r="B29" s="60" t="s">
         <v>37</v>
       </c>
@@ -5524,7 +4661,7 @@
       <c r="K29" s="64"/>
       <c r="L29" s="65"/>
       <c r="M29" s="65"/>
-      <c r="N29" s="151"/>
+      <c r="N29" s="150"/>
       <c r="O29" s="64"/>
       <c r="P29" s="65"/>
       <c r="Q29" s="11"/>
@@ -5541,144 +4678,82 @@
       <c r="AB29" s="10"/>
     </row>
     <row r="30" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="198" t="s">
+      <c r="A30" s="197" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="53" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="128" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="D30" s="129"/>
       <c r="E30" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="131"/>
-      <c r="G30" s="128" t="s">
-        <v>48</v>
-      </c>
+      <c r="F30" s="131">
+        <v>353</v>
+      </c>
+      <c r="G30" s="128"/>
       <c r="H30" s="130"/>
-      <c r="I30" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="I30" s="130"/>
       <c r="J30" s="132"/>
-      <c r="K30" s="128" t="s">
-        <v>48</v>
-      </c>
+      <c r="K30" s="128"/>
       <c r="L30" s="129"/>
-      <c r="M30" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="M30" s="130"/>
       <c r="N30" s="131"/>
-      <c r="O30" s="128" t="s">
-        <v>96</v>
-      </c>
+      <c r="O30" s="128"/>
       <c r="P30" s="129"/>
-      <c r="Q30" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="Q30" s="130"/>
       <c r="R30" s="132"/>
-      <c r="S30" s="133" t="s">
-        <v>96</v>
-      </c>
+      <c r="S30" s="133"/>
       <c r="T30" s="129"/>
-      <c r="U30" s="130" t="s">
-        <v>35</v>
-      </c>
+      <c r="U30" s="130"/>
       <c r="V30" s="130"/>
-      <c r="W30" s="153" t="s">
-        <v>48</v>
-      </c>
-      <c r="X30" s="129" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y30" s="129" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z30" s="154">
-        <v>457</v>
-      </c>
+      <c r="W30" s="152"/>
+      <c r="X30" s="129"/>
+      <c r="Y30" s="129"/>
+      <c r="Z30" s="153"/>
       <c r="AA30" s="68"/>
       <c r="AB30" s="10"/>
     </row>
     <row r="31" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="206"/>
+      <c r="A31" s="205"/>
       <c r="B31" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="58" t="s">
-        <v>181</v>
+      <c r="C31" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="E31" s="24" t="s">
         <v>33</v>
       </c>
       <c r="F31" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="H31" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="I31" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="J31" s="113" t="s">
-        <v>168</v>
-      </c>
-      <c r="K31" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="L31" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="M31" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="N31" s="93">
-        <v>430</v>
-      </c>
-      <c r="O31" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="P31" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q31" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="R31" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="S31" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="T31" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="U31" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="V31" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="W31" s="165" t="s">
-        <v>71</v>
-      </c>
-      <c r="X31" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y31" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z31" s="96">
-        <v>561</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="G31" s="20"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="113"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="93"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="66"/>
+      <c r="S31" s="58"/>
+      <c r="T31" s="24"/>
+      <c r="U31" s="24"/>
+      <c r="V31" s="66"/>
+      <c r="W31" s="164"/>
+      <c r="X31" s="25"/>
+      <c r="Y31" s="25"/>
+      <c r="Z31" s="96"/>
       <c r="AA31" s="68"/>
       <c r="AB31" s="10"/>
       <c r="AC31" s="78"/>
@@ -5686,62 +4761,38 @@
       <c r="AE31" s="78"/>
     </row>
     <row r="32" spans="1:31" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="199"/>
+      <c r="A32" s="198"/>
       <c r="B32" s="70" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="E32" s="22" t="s">
         <v>35</v>
       </c>
       <c r="F32" s="113" t="s">
-        <v>162</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="H32" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="I32" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="J32" s="115">
-        <v>351</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="G32" s="20"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="115"/>
       <c r="K32" s="54"/>
       <c r="L32" s="25"/>
       <c r="M32" s="25"/>
       <c r="N32" s="108"/>
-      <c r="O32" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="P32" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q32" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="R32" s="113" t="s">
-        <v>162</v>
-      </c>
-      <c r="S32" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="T32" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="U32" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="V32" s="113" t="s">
-        <v>162</v>
-      </c>
+      <c r="O32" s="20"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="113"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="22"/>
+      <c r="V32" s="113"/>
       <c r="W32" s="54"/>
       <c r="X32" s="22"/>
       <c r="Y32" s="22"/>
@@ -5753,15 +4804,15 @@
       <c r="AE32" s="78"/>
     </row>
     <row r="33" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="199"/>
+      <c r="A33" s="198"/>
       <c r="B33" s="59" t="s">
         <v>28</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>178</v>
+        <v>99</v>
       </c>
       <c r="E33" s="22" t="s">
         <v>33</v>
@@ -5777,49 +4828,31 @@
       <c r="L33" s="25"/>
       <c r="M33" s="25"/>
       <c r="N33" s="93"/>
-      <c r="O33" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="P33" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q33" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="R33" s="113">
-        <v>424</v>
-      </c>
-      <c r="S33" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="T33" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="U33" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="V33" s="113">
-        <v>424</v>
-      </c>
+      <c r="O33" s="20"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="113"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="22"/>
+      <c r="V33" s="113"/>
       <c r="W33" s="58"/>
       <c r="X33" s="22"/>
       <c r="Y33" s="24"/>
-      <c r="Z33" s="113" t="s">
-        <v>164</v>
-      </c>
+      <c r="Z33" s="113"/>
       <c r="AA33" s="68"/>
       <c r="AB33" s="78"/>
     </row>
     <row r="34" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="199"/>
+      <c r="A34" s="198"/>
       <c r="B34" s="59" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>151</v>
+        <v>93</v>
       </c>
       <c r="E34" s="22" t="s">
         <v>35</v>
@@ -5851,7 +4884,7 @@
       <c r="AB34" s="10"/>
     </row>
     <row r="35" spans="1:28" s="55" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="201"/>
+      <c r="A35" s="200"/>
       <c r="B35" s="60" t="s">
         <v>37</v>
       </c>
@@ -5877,13 +4910,13 @@
       <c r="V35" s="65"/>
       <c r="W35" s="58"/>
       <c r="X35" s="24"/>
-      <c r="Y35" s="159"/>
+      <c r="Y35" s="158"/>
       <c r="Z35" s="95"/>
       <c r="AA35" s="68"/>
       <c r="AB35" s="10"/>
     </row>
     <row r="36" spans="1:28" s="55" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="198" t="s">
+      <c r="A36" s="197" t="s">
         <v>32</v>
       </c>
       <c r="B36" s="53" t="s">
@@ -5909,23 +4942,15 @@
       <c r="T36" s="21"/>
       <c r="U36" s="21"/>
       <c r="V36" s="21"/>
-      <c r="W36" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="X36" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y36" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z36" s="117">
-        <v>536</v>
-      </c>
+      <c r="W36" s="23"/>
+      <c r="X36" s="21"/>
+      <c r="Y36" s="21"/>
+      <c r="Z36" s="117"/>
       <c r="AA36" s="68"/>
       <c r="AB36" s="10"/>
     </row>
     <row r="37" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="199"/>
+      <c r="A37" s="198"/>
       <c r="B37" s="59" t="s">
         <v>26</v>
       </c>
@@ -5933,30 +4958,14 @@
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
       <c r="F37" s="93"/>
-      <c r="G37" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="H37" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="I37" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="J37" s="113">
-        <v>330</v>
-      </c>
-      <c r="K37" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="L37" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="M37" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="N37" s="93">
-        <v>330</v>
-      </c>
+      <c r="G37" s="20"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="113"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="93"/>
       <c r="O37" s="58"/>
       <c r="P37" s="22"/>
       <c r="Q37" s="24"/>
@@ -5965,77 +4974,53 @@
       <c r="T37" s="22"/>
       <c r="U37" s="24"/>
       <c r="V37" s="25"/>
-      <c r="W37" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="X37" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y37" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z37" s="113">
-        <v>536</v>
-      </c>
+      <c r="W37" s="20"/>
+      <c r="X37" s="22"/>
+      <c r="Y37" s="22"/>
+      <c r="Z37" s="113"/>
       <c r="AA37" s="68"/>
       <c r="AB37" s="10"/>
     </row>
     <row r="38" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="199"/>
+      <c r="A38" s="198"/>
       <c r="B38" s="59" t="s">
         <v>27</v>
       </c>
       <c r="C38" s="87" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="D38" s="88"/>
       <c r="E38" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="F38" s="105"/>
-      <c r="G38" s="87" t="s">
-        <v>77</v>
-      </c>
+      <c r="F38" s="105" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" s="87"/>
       <c r="H38" s="88"/>
-      <c r="I38" s="89" t="s">
-        <v>35</v>
-      </c>
+      <c r="I38" s="89"/>
       <c r="J38" s="122"/>
-      <c r="K38" s="87" t="s">
-        <v>77</v>
-      </c>
+      <c r="K38" s="87"/>
       <c r="L38" s="88"/>
       <c r="M38" s="89"/>
       <c r="N38" s="105"/>
-      <c r="O38" s="87" t="s">
-        <v>77</v>
-      </c>
+      <c r="O38" s="87"/>
       <c r="P38" s="88"/>
-      <c r="Q38" s="89" t="s">
-        <v>35</v>
-      </c>
+      <c r="Q38" s="89"/>
       <c r="R38" s="118"/>
-      <c r="S38" s="87" t="s">
-        <v>77</v>
-      </c>
+      <c r="S38" s="87"/>
       <c r="T38" s="88"/>
-      <c r="U38" s="89" t="s">
-        <v>35</v>
-      </c>
+      <c r="U38" s="89"/>
       <c r="V38" s="89"/>
-      <c r="W38" s="87" t="s">
-        <v>77</v>
-      </c>
+      <c r="W38" s="87"/>
       <c r="X38" s="137"/>
-      <c r="Y38" s="134" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z38" s="139"/>
+      <c r="Y38" s="134"/>
+      <c r="Z38" s="138"/>
       <c r="AA38" s="68"/>
       <c r="AB38" s="10"/>
     </row>
     <row r="39" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="199"/>
+      <c r="A39" s="198"/>
       <c r="B39" s="59" t="s">
         <v>28</v>
       </c>
@@ -6043,9 +5028,7 @@
       <c r="D39" s="73"/>
       <c r="E39" s="22"/>
       <c r="F39" s="93"/>
-      <c r="G39" s="20" t="s">
-        <v>139</v>
-      </c>
+      <c r="G39" s="20"/>
       <c r="H39" s="73"/>
       <c r="I39" s="22"/>
       <c r="J39" s="113"/>
@@ -6053,15 +5036,11 @@
       <c r="L39" s="73"/>
       <c r="M39" s="22"/>
       <c r="N39" s="93"/>
-      <c r="O39" s="20" t="s">
-        <v>139</v>
-      </c>
+      <c r="O39" s="20"/>
       <c r="P39" s="73"/>
       <c r="Q39" s="22"/>
       <c r="R39" s="113"/>
-      <c r="S39" s="20" t="s">
-        <v>139</v>
-      </c>
+      <c r="S39" s="20"/>
       <c r="T39" s="73"/>
       <c r="U39" s="22"/>
       <c r="V39" s="22"/>
@@ -6073,28 +5052,28 @@
       <c r="AB39" s="10"/>
     </row>
     <row r="40" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="200"/>
+      <c r="A40" s="199"/>
       <c r="B40" s="60" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="58"/>
-      <c r="D40" s="197"/>
+      <c r="D40" s="196"/>
       <c r="E40" s="24"/>
       <c r="F40" s="66"/>
       <c r="G40" s="58"/>
-      <c r="H40" s="197"/>
+      <c r="H40" s="196"/>
       <c r="I40" s="24"/>
       <c r="J40" s="70"/>
       <c r="K40" s="71"/>
-      <c r="L40" s="197"/>
+      <c r="L40" s="196"/>
       <c r="M40" s="24"/>
       <c r="N40" s="66"/>
       <c r="O40" s="58"/>
-      <c r="P40" s="197"/>
+      <c r="P40" s="196"/>
       <c r="Q40" s="24"/>
       <c r="R40" s="70"/>
       <c r="S40" s="71"/>
-      <c r="T40" s="197"/>
+      <c r="T40" s="196"/>
       <c r="U40" s="24"/>
       <c r="V40" s="24"/>
       <c r="W40" s="58"/>
@@ -6105,7 +5084,7 @@
       <c r="AB40" s="10"/>
     </row>
     <row r="41" spans="1:28" s="55" customFormat="1" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="201"/>
+      <c r="A41" s="200"/>
       <c r="B41" s="60" t="s">
         <v>37</v>
       </c>
@@ -6152,19 +5131,19 @@
       <c r="K42" s="7"/>
       <c r="L42" s="7"/>
       <c r="M42" s="7"/>
-      <c r="N42" s="193"/>
+      <c r="N42" s="192"/>
       <c r="O42" s="6"/>
       <c r="P42" s="6"/>
       <c r="Q42" s="8"/>
-      <c r="R42" s="169"/>
+      <c r="R42" s="168"/>
       <c r="S42" s="6"/>
       <c r="T42" s="6"/>
       <c r="U42" s="8"/>
-      <c r="V42" s="178"/>
+      <c r="V42" s="177"/>
       <c r="W42" s="31"/>
       <c r="X42" s="31"/>
       <c r="Y42" s="31"/>
-      <c r="Z42" s="160"/>
+      <c r="Z42" s="159"/>
       <c r="AA42" s="85"/>
       <c r="AB42" s="10"/>
     </row>
@@ -6172,7 +5151,7 @@
       <c r="AB43" s="46"/>
     </row>
     <row r="53" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K53" s="194" t="s">
+      <c r="K53" s="193" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>